<commit_message>
chore: update raw Excel file
</commit_message>
<xml_diff>
--- a/data/raw/ruptura_database.xlsx
+++ b/data/raw/ruptura_database.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Downloads\VS_Code\Projetos e Estudos\- PROCESSO SELETIVO - PREPARAÇÃO\12. Cases Técnicos\case_gb\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKSPACE\etl_ruptura_zero\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0F8E62-C17E-48C5-8437-D7B8E9155BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2C005F-6CA8-4579-9A1B-38DF0EACAC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="01_BD_Ruptura_Faltaproduto" sheetId="1" r:id="rId1"/>
+    <sheet name="01_BD_Ruptura" sheetId="1" r:id="rId1"/>
     <sheet name="02_BD_Estoque" sheetId="2" r:id="rId2"/>
     <sheet name="03_BD_Vendas" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'01_BD_Ruptura_Faltaproduto'!$A$1:$H$1444</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'01_BD_Ruptura'!$A$1:$H$1444</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'02_BD_Estoque'!$A$1:$I$1398</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'03_BD_Vendas'!$A$1:$F$117</definedName>
   </definedNames>
@@ -7926,6 +7926,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -8191,7 +8192,7 @@
   </sheetPr>
   <dimension ref="A1:J1444"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
@@ -45770,7 +45771,7 @@
     <col min="4" max="4" width="25.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2571</v>
       </c>
@@ -45799,7 +45800,7 @@
         <v>2578</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2579</v>
       </c>
@@ -45828,7 +45829,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2579</v>
       </c>
@@ -45857,7 +45858,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2579</v>
       </c>
@@ -45886,7 +45887,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2579</v>
       </c>
@@ -45915,7 +45916,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2579</v>
       </c>
@@ -45944,7 +45945,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2579</v>
       </c>
@@ -45973,7 +45974,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46002,7 +46003,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46031,7 +46032,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46060,7 +46061,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46089,7 +46090,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46118,7 +46119,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46147,7 +46148,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46176,7 +46177,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46205,7 +46206,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46234,7 +46235,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46263,7 +46264,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46292,7 +46293,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46321,7 +46322,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46350,7 +46351,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46379,7 +46380,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46408,7 +46409,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46437,7 +46438,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46466,7 +46467,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46495,7 +46496,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46524,7 +46525,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46553,7 +46554,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46582,7 +46583,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46611,7 +46612,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46640,7 +46641,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46669,7 +46670,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46698,7 +46699,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46727,7 +46728,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46756,7 +46757,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46785,7 +46786,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46814,7 +46815,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46843,7 +46844,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46872,7 +46873,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46901,7 +46902,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>2579</v>
       </c>
@@ -46930,7 +46931,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>2579</v>
       </c>
@@ -86326,14 +86327,14 @@
   </sheetPr>
   <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -86353,7 +86354,7 @@
         <v>2598</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>202102</v>
       </c>
@@ -86373,7 +86374,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>202101</v>
       </c>
@@ -86393,7 +86394,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>202104</v>
       </c>
@@ -86413,7 +86414,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>202106</v>
       </c>
@@ -86433,7 +86434,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>202103</v>
       </c>
@@ -86453,7 +86454,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>202105</v>
       </c>
@@ -86473,7 +86474,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>202107</v>
       </c>
@@ -86493,7 +86494,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>202108</v>
       </c>
@@ -86513,7 +86514,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>202106</v>
       </c>
@@ -86533,7 +86534,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>202105</v>
       </c>
@@ -86553,7 +86554,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>202102</v>
       </c>
@@ -86573,7 +86574,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>202107</v>
       </c>
@@ -86593,7 +86594,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>202108</v>
       </c>
@@ -86613,7 +86614,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>202101</v>
       </c>
@@ -86633,7 +86634,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>202103</v>
       </c>
@@ -86653,7 +86654,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>202104</v>
       </c>
@@ -86673,7 +86674,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>202105</v>
       </c>
@@ -86693,7 +86694,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>202108</v>
       </c>
@@ -86713,7 +86714,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>202102</v>
       </c>
@@ -86733,7 +86734,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>202103</v>
       </c>
@@ -86753,7 +86754,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>202101</v>
       </c>
@@ -86773,7 +86774,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>202106</v>
       </c>
@@ -86793,7 +86794,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>202104</v>
       </c>
@@ -86813,7 +86814,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>202107</v>
       </c>
@@ -86833,7 +86834,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>202103</v>
       </c>
@@ -86853,7 +86854,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>202105</v>
       </c>
@@ -86873,7 +86874,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>202107</v>
       </c>
@@ -86893,7 +86894,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>202101</v>
       </c>
@@ -86913,7 +86914,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>202106</v>
       </c>
@@ -86933,7 +86934,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>202102</v>
       </c>
@@ -86953,7 +86954,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>202104</v>
       </c>
@@ -86973,7 +86974,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>202108</v>
       </c>
@@ -86993,7 +86994,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>202107</v>
       </c>
@@ -87013,7 +87014,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>202108</v>
       </c>
@@ -87033,7 +87034,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>202101</v>
       </c>
@@ -87053,7 +87054,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>202105</v>
       </c>
@@ -87073,7 +87074,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>202106</v>
       </c>
@@ -87093,7 +87094,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>202103</v>
       </c>
@@ -87113,7 +87114,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>202102</v>
       </c>
@@ -87133,7 +87134,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>202104</v>
       </c>

</xml_diff>